<commit_message>
Last Fix with Mush don't trivial Rounded
</commit_message>
<xml_diff>
--- a/Table1.xlsx
+++ b/Table1.xlsx
@@ -108,9 +108,18 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="3">
+  <x:cellStyleXfs count="6">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -485,7 +494,7 @@
       <x:c r="D2" s="2" t="s"/>
       <x:c r="E2" s="2" t="s"/>
       <x:c r="F2" s="2" t="n">
-        <x:v>1125</x:v>
+        <x:v>1161.29</x:v>
       </x:c>
       <x:c r="G2" s="2" t="n">
         <x:v>1936.492</x:v>
@@ -516,7 +525,7 @@
       <x:c r="D3" s="2" t="s"/>
       <x:c r="E3" s="2" t="s"/>
       <x:c r="F3" s="2" t="n">
-        <x:v>1104.706</x:v>
+        <x:v>1085.549</x:v>
       </x:c>
       <x:c r="G3" s="2" t="n">
         <x:v>488.688</x:v>
@@ -545,7 +554,7 @@
         <x:v>1.7</x:v>
       </x:c>
       <x:c r="D4" s="2" t="n">
-        <x:v>992.647</x:v>
+        <x:v>1024.668</x:v>
       </x:c>
       <x:c r="E4" s="2" t="n">
         <x:v>1117.245</x:v>
@@ -576,7 +585,7 @@
         <x:v>1.6585</x:v>
       </x:c>
       <x:c r="D5" s="2" t="n">
-        <x:v>942.914</x:v>
+        <x:v>926.563</x:v>
       </x:c>
       <x:c r="E5" s="2" t="n">
         <x:v>4049.736</x:v>
@@ -609,7 +618,7 @@
       <x:c r="D6" s="2" t="s"/>
       <x:c r="E6" s="2" t="s"/>
       <x:c r="F6" s="2" t="n">
-        <x:v>937.5</x:v>
+        <x:v>967.742</x:v>
       </x:c>
       <x:c r="G6" s="2" t="n">
         <x:v>1332.479</x:v>
@@ -638,7 +647,7 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D7" s="2" t="n">
-        <x:v>1250</x:v>
+        <x:v>1290.323</x:v>
       </x:c>
       <x:c r="E7" s="2" t="n">
         <x:v>774.597</x:v>
@@ -646,16 +655,16 @@
       <x:c r="F7" s="2" t="s"/>
       <x:c r="G7" s="2" t="s"/>
       <x:c r="H7" s="2" t="n">
-        <x:v>1.25</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="I7" s="2" t="n">
-        <x:v>1.25</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="J7" s="2" t="n">
-        <x:v>1.45</x:v>
+        <x:v>1.5</x:v>
       </x:c>
       <x:c r="K7" s="2" t="n">
-        <x:v>1.813</x:v>
+        <x:v>1.95</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:11">
@@ -671,22 +680,22 @@
       <x:c r="D8" s="2" t="s"/>
       <x:c r="E8" s="2" t="s"/>
       <x:c r="F8" s="2" t="n">
-        <x:v>731.706</x:v>
+        <x:v>719.017</x:v>
       </x:c>
       <x:c r="G8" s="2" t="n">
-        <x:v>98.772</x:v>
+        <x:v>276.563</x:v>
       </x:c>
       <x:c r="H8" s="2" t="n">
-        <x:v>3.1</x:v>
+        <x:v>2.9</x:v>
       </x:c>
       <x:c r="I8" s="2" t="n">
-        <x:v>0.75</x:v>
+        <x:v>0.7</x:v>
       </x:c>
       <x:c r="J8" s="2" t="n">
-        <x:v>0.95</x:v>
+        <x:v>0.9</x:v>
       </x:c>
       <x:c r="K8" s="2" t="n">
-        <x:v>2.945</x:v>
+        <x:v>2.61</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:11">
@@ -700,7 +709,7 @@
         <x:v>1.7</x:v>
       </x:c>
       <x:c r="D9" s="2" t="n">
-        <x:v>992.647</x:v>
+        <x:v>1024.668</x:v>
       </x:c>
       <x:c r="E9" s="2" t="n">
         <x:v>1117.245</x:v>
@@ -731,7 +740,7 @@
         <x:v>1.6585</x:v>
       </x:c>
       <x:c r="D10" s="2" t="n">
-        <x:v>942.914</x:v>
+        <x:v>926.563</x:v>
       </x:c>
       <x:c r="E10" s="2" t="n">
         <x:v>4049.736</x:v>
@@ -764,7 +773,7 @@
       <x:c r="D11" s="2" t="s"/>
       <x:c r="E11" s="2" t="s"/>
       <x:c r="F11" s="2" t="n">
-        <x:v>937.5</x:v>
+        <x:v>967.742</x:v>
       </x:c>
       <x:c r="G11" s="2" t="n">
         <x:v>1332.479</x:v>
@@ -795,22 +804,22 @@
       <x:c r="D12" s="2" t="s"/>
       <x:c r="E12" s="2" t="s"/>
       <x:c r="F12" s="2" t="n">
-        <x:v>1041.688</x:v>
+        <x:v>1075.29</x:v>
       </x:c>
       <x:c r="G12" s="2" t="n">
         <x:v>194.084</x:v>
       </x:c>
       <x:c r="H12" s="2" t="n">
-        <x:v>1.6</x:v>
+        <x:v>1.65</x:v>
       </x:c>
       <x:c r="I12" s="2" t="n">
-        <x:v>1.05</x:v>
+        <x:v>1.1</x:v>
       </x:c>
       <x:c r="J12" s="2" t="n">
-        <x:v>1.25</x:v>
+        <x:v>1.3</x:v>
       </x:c>
       <x:c r="K12" s="2" t="n">
-        <x:v>2</x:v>
+        <x:v>2.145</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:11">
@@ -824,7 +833,7 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="D13" s="2" t="n">
-        <x:v>729.167</x:v>
+        <x:v>752.688</x:v>
       </x:c>
       <x:c r="E13" s="2" t="n">
         <x:v>322.749</x:v>
@@ -855,7 +864,7 @@
         <x:v>2.439</x:v>
       </x:c>
       <x:c r="D14" s="2" t="n">
-        <x:v>829.414</x:v>
+        <x:v>815.031</x:v>
       </x:c>
       <x:c r="E14" s="2" t="n">
         <x:v>1012.428</x:v>

</xml_diff>